<commit_message>
Lösche Kurs in Zeile 10
</commit_message>
<xml_diff>
--- a/Usi-kurse.xlsx
+++ b/Usi-kurse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ingrid\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ingrid\Documents\GitHub\LC-GitHub-Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14A78B35-F8F0-453B-8CAD-B103A87C6E60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D2635D-32F7-4150-812D-28AB6121D8FD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{33A72481-4243-4EDC-AF8E-61EC5CF79778}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Kurs</t>
   </si>
@@ -118,15 +118,6 @@
   </si>
   <si>
     <t>911</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPITALGASSE </t>
-  </si>
-  <si>
-    <t>2050 - 2157</t>
-  </si>
-  <si>
-    <t>Giesswein Volker</t>
   </si>
 </sst>
 </file>
@@ -179,10 +170,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -195,15 +189,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -520,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6558A182-0C42-4DAD-A306-2E2C9F2B9E62}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L10"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +518,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -570,35 +555,35 @@
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>41</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="3">
         <v>60</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="3">
         <v>2</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -606,23 +591,23 @@
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>1504</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -631,82 +616,82 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="3">
         <v>60</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <v>28</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>363</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>43222</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="3">
         <v>60</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <v>47</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7" t="s">
+      <c r="K6" s="3"/>
+      <c r="L6" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -714,51 +699,51 @@
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>43222</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <v>60</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <v>45</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -766,78 +751,32 @@
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2">
-        <v>391</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="4">
-        <v>43221</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="2">
-        <v>60</v>
-      </c>
-      <c r="I10" s="2">
-        <v>27</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
@@ -847,18 +786,28 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://www.usi.at/de/sportstaetten/brg14" xr:uid="{9F5FC138-3AE0-45CD-BDAB-C858A00EB891}"/>
@@ -873,11 +822,8 @@
     <hyperlink ref="F8" r:id="rId10" display="https://www.usi.at/de/sportstaetten/brg14" xr:uid="{2779744F-C6DD-4C57-A8FF-B5C0BD0504C7}"/>
     <hyperlink ref="J8" r:id="rId11" location="!/lehrer/1324" display="https://www.usi.at/de/angebot/ - !/lehrer/1324" xr:uid="{94204C63-BCB2-458F-9EF6-7C9F6C55D1A5}"/>
     <hyperlink ref="L8" r:id="rId12" display="https://www.usi-wien.at/anmeldung/secure/course/911?show" xr:uid="{7A96CC68-2103-4CD8-B82A-397E79AE55CF}"/>
-    <hyperlink ref="F10" r:id="rId13" display="https://www.usi.at/de/sportstaetten/spitalgasse" xr:uid="{0E625328-71D5-453C-BAE1-A32D667FFC78}"/>
-    <hyperlink ref="J10" r:id="rId14" location="!/lehrer/800" display="https://www.usi.at/de/angebot/ - !/lehrer/800" xr:uid="{6443052E-3146-42B8-87CE-C1679D71DFBA}"/>
-    <hyperlink ref="L10" r:id="rId15" display="https://www.usi-wien.at/anmeldung/secure/course/391?show" xr:uid="{6D369615-6959-42BF-8306-DD40E71D3658}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>